<commit_message>
Fix sell report of AMD and added preperations for next week
</commit_message>
<xml_diff>
--- a/Start Your Own/preperations for next week.xlsx
+++ b/Start Your Own/preperations for next week.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oferg/work/mycode/ChatGPT-Micro-Cap-Experiment/Start Your Own/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3C6DCEA-3B46-774C-8CD3-6AAF11C64841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A10123A-A614-6F47-8828-965E37154449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="34560" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Ticker</t>
   </si>
@@ -37,50 +37,26 @@
     <t>New Portfolio %</t>
   </si>
   <si>
-    <t>IBIT</t>
-  </si>
-  <si>
     <t>SELL</t>
   </si>
   <si>
-    <t>CWCO</t>
-  </si>
-  <si>
-    <t>ASML</t>
-  </si>
-  <si>
-    <t>CRWD</t>
-  </si>
-  <si>
-    <t>IREN</t>
-  </si>
-  <si>
     <t>AMD</t>
   </si>
   <si>
     <t>BUY</t>
   </si>
   <si>
-    <t>BE</t>
-  </si>
-  <si>
-    <t>AVGO</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>RESULT</t>
-  </si>
-  <si>
-    <t>N/A</t>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>PLTR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -91,6 +67,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -114,10 +104,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,9 +330,14 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
@@ -360,159 +357,88 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
+      <c r="C2" s="4">
+        <v>0.1605</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1.7824</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
+      <c r="C3" s="4">
+        <v>0.14291000000000001</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7.8100000000000003E-2</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.43159999999999998</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.2</v>
-      </c>
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.16947000000000001</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1">
-        <v>1.2506999999999999</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.89649999999999996</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.79249999999999998</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2.8633000000000002</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1">
-        <v>4.1000000000000003E-3</v>
-      </c>
-      <c r="D7" s="1">
-        <v>3.3323999999999998</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>6.8773</v>
-      </c>
-      <c r="D8" s="1">
-        <v>6.8773</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0.59060000000000001</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.59060000000000001</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>